<commit_message>
pinout and invoice added
</commit_message>
<xml_diff>
--- a/Dokumentacja_projektu/Kosztorys/Zamowione_elementy/Zamówienia.xlsx
+++ b/Dokumentacja_projektu/Kosztorys/Zamowione_elementy/Zamówienia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\DC-DC_Converter_Tester\Dokumentacja_projektu\Kosztorys\Zamowione_elementy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF96F17-E2A4-4B67-AE1F-4BCFF9411C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36037C5-7C96-4204-AEC8-B5F3E3FEB180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>SKLEP</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>PCB Panele frontowe</t>
+  </si>
+  <si>
+    <t>AV-Elektronika</t>
+  </si>
+  <si>
+    <t>Części do mainboard'a</t>
   </si>
 </sst>
 </file>
@@ -355,6 +361,15 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -362,15 +377,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -390,7 +396,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{58B71C8B-F6E5-4223-87F2-612BE4736AEF}" name="Tabela1" displayName="Tabela1" ref="B2:D45" totalsRowShown="0" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{58B71C8B-F6E5-4223-87F2-612BE4736AEF}" name="Tabela1" displayName="Tabela1" ref="B2:D45" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="B2:D45" xr:uid="{58B71C8B-F6E5-4223-87F2-612BE4736AEF}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{22E1A9CB-8528-4AE0-AF96-775700D0DA31}" name="OPIS" dataDxfId="2"/>
@@ -667,7 +673,7 @@
   <dimension ref="B2:H45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,7 +729,7 @@
       </c>
       <c r="H4" s="12">
         <f>SUM(Tabela1[KWOTA PLN])</f>
-        <v>1679.7399999999998</v>
+        <v>1981.9799999999998</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -839,14 +845,26 @@
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="8"/>
+      <c r="B15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="8">
+        <v>24.5</v>
+      </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="8"/>
+      <c r="B16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="8">
+        <v>277.74</v>
+      </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>

</xml_diff>